<commit_message>
Make sure that row indices are strings
</commit_message>
<xml_diff>
--- a/test/data/metabolite.xlsx
+++ b/test/data/metabolite.xlsx
@@ -30,13 +30,13 @@
     <t>instance_4</t>
   </si>
   <si>
-    <t>Met1</t>
-  </si>
-  <si>
-    <t>Met2</t>
-  </si>
-  <si>
-    <t>Met3</t>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
   <si>
     <t>NaN</t>

</xml_diff>